<commit_message>
excel and csv update
</commit_message>
<xml_diff>
--- a/productListingxlsx.xlsx
+++ b/productListingxlsx.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Website-Backup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vince\Documents\Website-Backup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C529136-6005-4AB4-9E59-A044AD743CAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DB97F8-52A1-450F-BB0A-D9B940ECFA16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D935BBD5-3674-47DB-A6F1-94EDAC206A22}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{D935BBD5-3674-47DB-A6F1-94EDAC206A22}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -90,12 +90,6 @@
     <t>productImages/Black Sweater.jpeg</t>
   </si>
   <si>
-    <t>productImages/Red Jacket.jpeg</t>
-  </si>
-  <si>
-    <t>productImages/White Shirt.jpeg</t>
-  </si>
-  <si>
     <t>productImages/Blue Shirt.jpeg</t>
   </si>
   <si>
@@ -121,6 +115,12 @@
   </si>
   <si>
     <t>Sweater</t>
+  </si>
+  <si>
+    <t>https://github.com/Vincent-Cayadi/Website-Backup/blob/main/productImages/Black%20Sweater.jpeg</t>
+  </si>
+  <si>
+    <t>https://github.com/Vincent-Cayadi/Website-Backup/blob/main/productImages/White%20Shirt.jpeg</t>
   </si>
 </sst>
 </file>
@@ -490,24 +490,24 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="21" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.1796875" style="2"/>
+    <col min="9" max="9" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -536,7 +536,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -544,13 +544,13 @@
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H2" s="2">
         <v>100000000000000</v>
@@ -559,7 +559,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -567,10 +567,10 @@
         <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H3" s="2">
         <v>100000000000000</v>
@@ -579,7 +579,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -590,7 +590,7 @@
         <v>19</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H4" s="2">
         <v>100000000000000</v>
@@ -599,7 +599,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -607,10 +607,10 @@
         <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H5" s="2">
         <v>100000000000000</v>
@@ -619,7 +619,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -627,10 +627,10 @@
         <v>14</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H6" s="2">
         <v>100000000000000</v>
@@ -639,7 +639,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -647,10 +647,10 @@
         <v>16</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H7" s="2">
         <v>100000000000000</v>
@@ -659,7 +659,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -667,10 +667,10 @@
         <v>15</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H8" s="2">
         <v>100000000000000</v>
@@ -679,7 +679,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -687,11 +687,11 @@
         <v>17</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="H9" s="2">
         <v>100000000000000</v>
       </c>
@@ -699,7 +699,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -707,10 +707,10 @@
         <v>18</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H10" s="2">
         <v>100000000000000</v>

</xml_diff>

<commit_message>
Retriving Data From MongoDB works
Have to change the DB thingy
</commit_message>
<xml_diff>
--- a/productListingxlsx.xlsx
+++ b/productListingxlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vince\Documents\Website-Backup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C66101-242F-424B-814F-C4DB3D8D3CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB8DEE6-B806-4B7B-A175-9CAA86632191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{D935BBD5-3674-47DB-A6F1-94EDAC206A22}"/>
   </bookViews>
@@ -33,9 +33,6 @@
     <t>SKU</t>
   </si>
   <si>
-    <t xml:space="preserve">product name </t>
-  </si>
-  <si>
     <t>productPictureSmall</t>
   </si>
   <si>
@@ -202,6 +199,9 @@
   </si>
   <si>
     <t>https://github.com/Vincent-Cayadi/Website-Backup/blob/main/productImages/Ispark%20Pencil%20Case.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">productName </t>
   </si>
 </sst>
 </file>
@@ -579,7 +579,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -600,28 +600,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
       <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="I1" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.4">
@@ -629,17 +629,17 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4">
@@ -654,15 +654,15 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4">
@@ -677,15 +677,15 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4">
@@ -700,15 +700,15 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4">
@@ -723,15 +723,15 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4">
@@ -746,15 +746,15 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4">
@@ -769,15 +769,15 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4">
@@ -792,15 +792,15 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="4">
@@ -815,15 +815,15 @@
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4">
@@ -838,15 +838,15 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4">
@@ -861,15 +861,15 @@
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4">
@@ -884,15 +884,15 @@
         <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4">
@@ -907,15 +907,15 @@
         <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4">
@@ -930,15 +930,15 @@
         <v>13</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4">
@@ -953,15 +953,15 @@
         <v>14</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="4">
@@ -976,15 +976,15 @@
         <v>15</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G17" s="4"/>
       <c r="H17" s="4">
@@ -999,15 +999,15 @@
         <v>16</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="4">
@@ -1022,15 +1022,15 @@
         <v>17</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="4">
@@ -1045,15 +1045,15 @@
         <v>18</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4">
@@ -1068,15 +1068,15 @@
         <v>19</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="4">
@@ -1091,15 +1091,15 @@
         <v>20</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="4">
@@ -1114,15 +1114,15 @@
         <v>21</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="4">
@@ -1137,15 +1137,15 @@
         <v>22</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G24" s="4"/>
       <c r="H24" s="4">
@@ -1160,15 +1160,15 @@
         <v>23</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G25" s="4"/>
       <c r="H25" s="4">

</xml_diff>

<commit_message>
Finished getting the data from database
</commit_message>
<xml_diff>
--- a/productListingxlsx.xlsx
+++ b/productListingxlsx.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vince\Documents\Website-Backup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Website-Backup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{992A93E7-7D76-47AB-9AD5-8F9F5ED27C03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586D3A97-0B5F-4916-8828-80B00742B55A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{D935BBD5-3674-47DB-A6F1-94EDAC206A22}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D935BBD5-3674-47DB-A6F1-94EDAC206A22}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,10 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="54">
-  <si>
-    <t>SKU</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="60">
   <si>
     <t>price</t>
   </si>
@@ -186,10 +183,31 @@
     <t>https://github.com/Vincent-Cayadi/Website-Backup/blob/main/productImages/Ispark%20Pencil%20Case.jpg</t>
   </si>
   <si>
-    <t xml:space="preserve">productName </t>
-  </si>
-  <si>
-    <t>productPicture</t>
+    <t>img</t>
+  </si>
+  <si>
+    <t>name:</t>
+  </si>
+  <si>
+    <t>save</t>
+  </si>
+  <si>
+    <t>sizeInPage</t>
+  </si>
+  <si>
+    <t>sizeselected</t>
+  </si>
+  <si>
+    <t>itemInCart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">false  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">true </t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -564,55 +582,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05F00976-E28F-4968-82B1-C18C12768F15}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="21" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="229.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="8.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="229.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.90625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>52</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.4">
+      <c r="H1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" s="4">
         <v>20</v>
@@ -620,19 +652,31 @@
       <c r="F2" s="4">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.4">
+      <c r="G2" s="4">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="4">
         <v>20</v>
@@ -640,19 +684,28 @@
       <c r="F3" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.4">
+      <c r="G3" s="4">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="4">
         <v>20</v>
@@ -660,19 +713,28 @@
       <c r="F4" s="4">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.4">
+      <c r="G4" s="4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E5" s="4">
         <v>20</v>
@@ -680,19 +742,28 @@
       <c r="F5" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.4">
+      <c r="G5" s="4">
+        <v>0</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" s="4">
         <v>20</v>
@@ -700,19 +771,28 @@
       <c r="F6" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.4">
+      <c r="G6" s="4">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" s="4">
         <v>20</v>
@@ -720,19 +800,28 @@
       <c r="F7" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.4">
+      <c r="G7" s="4">
+        <v>0</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8" s="4">
         <v>20</v>
@@ -740,19 +829,28 @@
       <c r="F8" s="4">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.4">
+      <c r="G8" s="4">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="4">
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E9" s="4">
         <v>20</v>
@@ -760,19 +858,28 @@
       <c r="F9" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.4">
+      <c r="G9" s="4">
+        <v>0</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="4">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E10" s="4">
         <v>20</v>
@@ -780,19 +887,28 @@
       <c r="F10" s="4">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.4">
+      <c r="G10" s="4">
+        <v>0</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="4">
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E11" s="4">
         <v>20</v>
@@ -800,19 +916,28 @@
       <c r="F11" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.4">
+      <c r="G11" s="4">
+        <v>0</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="4">
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E12" s="4">
         <v>20</v>
@@ -820,19 +945,28 @@
       <c r="F12" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.4">
+      <c r="G12" s="4">
+        <v>0</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="4">
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E13" s="4">
         <v>20</v>
@@ -840,19 +974,28 @@
       <c r="F13" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.4">
+      <c r="G13" s="4">
+        <v>0</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="4">
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E14" s="4">
         <v>20</v>
@@ -860,19 +1003,28 @@
       <c r="F14" s="4">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.4">
+      <c r="G14" s="4">
+        <v>0</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="4">
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E15" s="4">
         <v>20</v>
@@ -880,19 +1032,28 @@
       <c r="F15" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.4">
+      <c r="G15" s="4">
+        <v>0</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="4">
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E16" s="4">
         <v>20</v>
@@ -900,19 +1061,28 @@
       <c r="F16" s="4">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.4">
+      <c r="G16" s="4">
+        <v>0</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="4">
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E17" s="4">
         <v>20</v>
@@ -920,19 +1090,28 @@
       <c r="F17" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.4">
+      <c r="G17" s="4">
+        <v>0</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="4">
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E18" s="4">
         <v>20</v>
@@ -940,19 +1119,28 @@
       <c r="F18" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.4">
+      <c r="G18" s="4">
+        <v>0</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="4">
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E19" s="4">
         <v>20</v>
@@ -960,19 +1148,28 @@
       <c r="F19" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.4">
+      <c r="G19" s="4">
+        <v>0</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="4">
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E20" s="4">
         <v>20</v>
@@ -980,19 +1177,28 @@
       <c r="F20" s="4">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.4">
+      <c r="G20" s="4">
+        <v>0</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="4">
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E21" s="4">
         <v>20</v>
@@ -1000,19 +1206,28 @@
       <c r="F21" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.4">
+      <c r="G21" s="4">
+        <v>0</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="4">
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E22" s="4">
         <v>20</v>
@@ -1020,19 +1235,28 @@
       <c r="F22" s="4">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.4">
+      <c r="G22" s="4">
+        <v>0</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="4">
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E23" s="4">
         <v>20</v>
@@ -1040,19 +1264,28 @@
       <c r="F23" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.4">
+      <c r="G23" s="4">
+        <v>0</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="4">
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E24" s="4">
         <v>20</v>
@@ -1060,25 +1293,43 @@
       <c r="F24" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.4">
+      <c r="G24" s="4">
+        <v>0</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="29.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="4">
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E25" s="4">
         <v>20</v>
       </c>
       <c r="F25" s="4">
         <v>15</v>
+      </c>
+      <c r="G25" s="4">
+        <v>0</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>